<commit_message>
FILI_WizardTest2504 : Changes to run script per jurisdiction
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EBF2FF-F2ED-4002-A160-A4AB2EC347C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091D04D9-421E-40ED-8D1E-7AA8DCB40D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="936" yWindow="936" windowWidth="17280" windowHeight="9108" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>Client Name</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Agent Module</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB77993-C7EC-411C-A1DE-F48C8A198BE7}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,13 +651,13 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -665,13 +668,13 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -682,13 +685,13 @@
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -699,13 +702,13 @@
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -716,13 +719,13 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -733,13 +736,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,13 +753,13 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -767,13 +770,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -784,17 +787,34 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E10">
+  <conditionalFormatting sqref="D2:E11">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -812,7 +832,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,15 +999,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005C83CA1A5F4AE4C9BEF6454A5CBD615" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec7417affe12c862527167136ce573ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xmlns:ns4="e178c8a6-526e-465c-b240-e7ca9adf772c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3e517818b1b2821051a10e8ea2fc5c" ns3:_="" ns4:_="">
     <xsd:import namespace="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
@@ -1220,6 +1231,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1229,14 +1249,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B973315-B0F0-4CE1-9BD5-E731C7EF6E1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1255,6 +1267,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
add the formated JSON
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091D04D9-421E-40ED-8D1E-7AA8DCB40D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA0AD58-7B0D-4CDE-8BB2-6BDF561EF001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="936" windowWidth="17280" windowHeight="9108" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>Client Name</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>JurisdictionWiseReport</t>
   </si>
 </sst>
 </file>
@@ -611,22 +614,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB77993-C7EC-411C-A1DE-F48C8A198BE7}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,8 +646,11 @@
       <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -659,8 +666,11 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -676,8 +686,11 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -693,8 +706,11 @@
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,8 +726,11 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -727,8 +746,11 @@
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -744,8 +766,11 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -761,8 +786,11 @@
       <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -776,10 +804,13 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -795,8 +826,11 @@
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -810,11 +844,14 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E11">
+  <conditionalFormatting sqref="D2:F11">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -835,15 +872,15 @@
       <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -857,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -871,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -885,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -899,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -914,7 +951,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -928,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -942,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -999,6 +1036,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005C83CA1A5F4AE4C9BEF6454A5CBD615" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec7417affe12c862527167136ce573ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xmlns:ns4="e178c8a6-526e-465c-b240-e7ca9adf772c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3e517818b1b2821051a10e8ea2fc5c" ns3:_="" ns4:_="">
     <xsd:import namespace="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
@@ -1231,7 +1276,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1240,15 +1285,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B973315-B0F0-4CE1-9BD5-E731C7EF6E1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1267,20 +1314,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to selenium 4.1.0
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C0F383-568A-4098-9A77-43107313CF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC960EC8-8288-419C-A5EA-792FA045D1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
@@ -617,7 +617,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
@@ -704,7 +704,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
@@ -724,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>4</v>
@@ -744,7 +744,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
@@ -764,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
@@ -784,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
@@ -804,10 +804,10 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Refactor Updated : Refactored Code pushed with upgraded selenium libraries
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C0F383-568A-4098-9A77-43107313CF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51407B02-E640-4DBD-A56E-C4F3A9FDCC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -617,20 +617,20 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -650,7 +650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -684,13 +684,13 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -704,13 +704,13 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -724,13 +724,13 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -744,13 +744,13 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -764,13 +764,13 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -784,13 +784,13 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -804,13 +804,13 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -827,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>4</v>
@@ -872,15 +872,15 @@
       <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -936,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +951,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -965,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1044,6 +1044,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005C83CA1A5F4AE4C9BEF6454A5CBD615" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec7417affe12c862527167136ce573ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xmlns:ns4="e178c8a6-526e-465c-b240-e7ca9adf772c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3e517818b1b2821051a10e8ea2fc5c" ns3:_="" ns4:_="">
     <xsd:import namespace="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
@@ -1276,15 +1285,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
   <ds:schemaRefs>
@@ -1296,6 +1296,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B973315-B0F0-4CE1-9BD5-E731C7EF6E1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1312,12 +1320,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Integrations : Code pushed to handle JSON changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51407B02-E640-4DBD-A56E-C4F3A9FDCC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E7FA0D-6E2C-458D-9BDA-F352F3061F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
   <si>
     <t>Client Name</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>JurisdictionWiseReport</t>
+  </si>
+  <si>
+    <t>SGB</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t>Direct Login</t>
   </si>
 </sst>
 </file>
@@ -211,13 +220,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,244 +624,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB77993-C7EC-411C-A1DE-F48C8A198BE7}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F11" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:F11">
+  <conditionalFormatting sqref="E2:G11">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -872,15 +1057,15 @@
       <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +1079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +1107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -936,7 +1121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +1136,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -965,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -979,7 +1164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1036,23 +1221,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005C83CA1A5F4AE4C9BEF6454A5CBD615" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec7417affe12c862527167136ce573ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xmlns:ns4="e178c8a6-526e-465c-b240-e7ca9adf772c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3e517818b1b2821051a10e8ea2fc5c" ns3:_="" ns4:_="">
     <xsd:import namespace="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
@@ -1285,25 +1453,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B973315-B0F0-4CE1-9BD5-E731C7EF6E1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1320,4 +1487,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code refactor and move cucumber to Allure
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51407B02-E640-4DBD-A56E-C4F3A9FDCC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60CB055-836C-437F-ACC7-8A50E2300A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -617,20 +617,20 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -650,7 +650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -690,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -750,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -770,7 +770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -790,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -810,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -830,7 +830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -844,10 +844,10 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -872,15 +872,15 @@
       <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -936,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +951,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -965,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1036,20 +1036,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1286,19 +1286,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
delete the temp file in system for make script faster
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60CB055-836C-437F-ACC7-8A50E2300A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26874A8-A986-49E0-8167-726238A7340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,20 +1036,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1286,19 +1286,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update the flow interface
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FlowInterface.xlsx
+++ b/src/test/resources/testdata/FlowInterface.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26874A8-A986-49E0-8167-726238A7340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996DFAE-CDD8-4584-8DFB-583AEB07D342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{181615CE-948B-4B1E-A394-A1F048FF8318}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="E2E" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,53 +37,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>Client Name</t>
   </si>
   <si>
-    <t>Inbound Type</t>
-  </si>
-  <si>
-    <t>SGB1</t>
-  </si>
-  <si>
-    <t>Tx103</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>HDFC</t>
-  </si>
-  <si>
-    <t>Foresight</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>Inbound</t>
-  </si>
-  <si>
-    <t>Outbound</t>
-  </si>
-  <si>
-    <t>NationalInsurance</t>
-  </si>
-  <si>
-    <t>BajajFinserv</t>
-  </si>
-  <si>
     <t>FILI</t>
   </si>
   <si>
-    <t>FBW</t>
-  </si>
-  <si>
     <t>Modules</t>
   </si>
   <si>
@@ -93,12 +60,6 @@
     <t>FILI.xlsx</t>
   </si>
   <si>
-    <t>MasterTemplate.xlsx</t>
-  </si>
-  <si>
-    <t>Owner Module, Trust Certification Module</t>
-  </si>
-  <si>
     <t>Execute</t>
   </si>
   <si>
@@ -139,20 +100,22 @@
   </si>
   <si>
     <t>JurisdictionWiseReport</t>
+  </si>
+  <si>
+    <t>E2EFlow.xlsx</t>
+  </si>
+  <si>
+    <t>Scenario1</t>
+  </si>
+  <si>
+    <t>Scenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,63 +170,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -617,7 +537,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,227 +555,227 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:F11">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -865,156 +785,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA9D55E-3BB1-4206-BB11-B87B369F4DDC}">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13A3B51-9C6E-49BC-9BAA-F92857EC427E}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C7">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D7">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9:E9">
+  <conditionalFormatting sqref="D2:E2">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1022,37 +843,11 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B7" xr:uid="{11725EC8-FF97-4788-94C3-752E539821C2}">
-      <formula1>"Tx103,Foresight,API"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D7" xr:uid="{1A3F24F9-E7F0-4E0F-BDF2-9A5DC2FA1AB7}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005C83CA1A5F4AE4C9BEF6454A5CBD615" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ec7417affe12c862527167136ce573ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xmlns:ns4="e178c8a6-526e-465c-b240-e7ca9adf772c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3e517818b1b2821051a10e8ea2fc5c" ns3:_="" ns4:_="">
     <xsd:import namespace="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
@@ -1285,25 +1080,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f905fdd-d228-4768-8e98-39c2c3fc93fc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B973315-B0F0-4CE1-9BD5-E731C7EF6E1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1320,4 +1114,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F607A51-1680-4B23-AACE-40B4CF7D53C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f905fdd-d228-4768-8e98-39c2c3fc93fc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28C1F0FE-A252-4DCA-9928-5CED55A2AC2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>